<commit_message>
BAL added, but refresh bug not resolved
</commit_message>
<xml_diff>
--- a/Data Source/Bill_data_summary.xlsx
+++ b/Data Source/Bill_data_summary.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saika\OneDrive\My Study\Design Patterns\Repository\Data Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saika\Documents\Visual Studio 2012\Projects\Repository_Pattern\Data Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="771F3A5FFCBF6C4E09A79053EDA5C2C53C44832A" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{BB219916-15D7-4732-A4D3-AEB1F5F7CA36}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{67990CDA-DD1B-4BBB-AD66-1A751965A13F}"/>
   </bookViews>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>BillId</t>
   </si>
@@ -76,6 +75,39 @@
   </si>
   <si>
     <t>Serena</t>
+  </si>
+  <si>
+    <t>BILL008</t>
+  </si>
+  <si>
+    <t>BILL009</t>
+  </si>
+  <si>
+    <t>BILL010</t>
+  </si>
+  <si>
+    <t>BILL011</t>
+  </si>
+  <si>
+    <t>BILL012</t>
+  </si>
+  <si>
+    <t>BILL013</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Gibson</t>
+  </si>
+  <si>
+    <t>Nagalingaraj</t>
+  </si>
+  <si>
+    <t>&lt;NULL&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bnull&gt;</t>
   </si>
 </sst>
 </file>
@@ -434,13 +466,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80984B8-6A20-4EA2-AFD8-BA2EF28E7273}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -554,6 +589,87 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>2344.67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>144.56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>2000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>1500</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>7544.08</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>